<commit_message>
v1.0 Initial WF Login Reviews with owner status
LH_WF_LOGIN_Create_005
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_LOGIN_REVIEWS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{898CD8BA-5EEE-482A-AEFF-AE1E4C08CCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C21F7-6F65-4929-8BFC-6FDF034865E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,6 @@
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -109,6 +108,9 @@
   </si>
   <si>
     <t>Add a “Forgot password?” link below the password field or near the Sign in button.</t>
+  </si>
+  <si>
+    <t>not applicable</t>
   </si>
 </sst>
 </file>
@@ -433,15 +435,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -458,6 +451,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -743,7 +745,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,7 +792,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -802,24 +804,24 @@
       <c r="D2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="32" t="s">
-        <v>20</v>
+      <c r="H2" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="24" t="s">
         <v>22</v>
       </c>
@@ -829,24 +831,24 @@
       <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>20</v>
+      <c r="H3" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="17" t="s">
         <v>23</v>
       </c>
@@ -856,17 +858,17 @@
       <c r="D4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="32" t="s">
-        <v>20</v>
+      <c r="H4" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>20</v>
@@ -982,7 +984,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
v1.1 The review comments Closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_LOGIN_REVIEWS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C21F7-6F65-4929-8BFC-6FDF034865E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BD2E3C-A172-46C0-8559-A64AACCF254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_Review_WF_LOGIN" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Mahmoud Rady</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>LH_Review_WF_LOGIN_001</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
   </si>
   <si>
     <t>not applicable</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The review comments Closed </t>
   </si>
 </sst>
 </file>
@@ -361,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -394,12 +400,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,205 +762,205 @@
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="30"/>
+      <c r="B3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="27" t="s">
+      <c r="E3" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H3" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="24" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="26" t="s">
+      <c r="E4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="F4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H4" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,10 +1024,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="10">
+        <v>45768</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
@@ -1036,6 +1044,7 @@
       <c r="D4" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.2 reopen task again to modify something
ask to add more details to registration form wireframe
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_LOGIN_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_LOGIN_REVIEWS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BD2E3C-A172-46C0-8559-A64AACCF254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C21F7-6F65-4929-8BFC-6FDF034865E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_Review_WF_LOGIN" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,9 @@
     <t>Mahmoud Rady</t>
   </si>
   <si>
+    <t>open</t>
+  </si>
+  <si>
     <t>LH_Review_WF_LOGIN_001</t>
   </si>
   <si>
@@ -108,15 +111,6 @@
   </si>
   <si>
     <t>not applicable</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The review comments Closed </t>
   </si>
 </sst>
 </file>
@@ -367,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -400,6 +394,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,205 +762,205 @@
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="25" t="s">
+      <c r="E3" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H3" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="G4" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>28</v>
+      <c r="I4" s="19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,18 +1024,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="10">
-        <v>45768</v>
-      </c>
+      <c r="A3" s="11"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
@@ -1044,7 +1036,6 @@
       <c r="D4" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>